<commit_message>
atualizando big chart conforme recomendado
</commit_message>
<xml_diff>
--- a/documentos/bigChart/BigChartProjeto.xlsx
+++ b/documentos/bigChart/BigChartProjeto.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="13300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Data</t>
   </si>
@@ -41,12 +41,15 @@
     <t>Páginas GSP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Controladoras</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -64,6 +67,11 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -101,6 +109,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,8 +123,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:lang val="pt-BR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -155,25 +165,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40443.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40457.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40471.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40485.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40499.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40513.0</c:v>
+                  <c:v>40499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -185,7 +198,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -232,25 +248,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40443.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40457.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40471.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40485.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40499.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40513.0</c:v>
+                  <c:v>40499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -262,7 +281,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -286,25 +308,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40443.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40457.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40471.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40485.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40499.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40513.0</c:v>
+                  <c:v>40499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -316,7 +341,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,25 +368,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40443.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40457.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40471.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40485.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40499.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40513.0</c:v>
+                  <c:v>40499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -370,7 +401,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>15.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,25 +428,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40443.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40457.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40471.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40485.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40499.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40513.0</c:v>
+                  <c:v>40499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -424,18 +461,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Controladoras</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="499882632"/>
-        <c:axId val="500232184"/>
+        <c:axId val="55630464"/>
+        <c:axId val="55512064"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="499882632"/>
+        <c:axId val="55630464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -450,21 +512,21 @@
             <a:pPr>
               <a:defRPr lang="pt-BR"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500232184"/>
+        <c:crossAx val="55512064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="14.0"/>
+        <c:majorUnit val="14"/>
         <c:majorTimeUnit val="days"/>
-        <c:minorUnit val="7.0"/>
+        <c:minorUnit val="7"/>
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="500232184"/>
+        <c:axId val="55512064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,10 +542,10 @@
             <a:pPr>
               <a:defRPr lang="pt-BR"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499882632"/>
+        <c:crossAx val="55630464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -499,7 +561,7 @@
             <a:pPr rtl="0">
               <a:defRPr lang="pt-BR"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -509,7 +571,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.984251969" l="0.787401575" r="0.787401575" t="0.984251969" header="0.492125985" footer="0.492125985"/>
+    <c:pageMargins b="0.98425196899999989" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999989" header="0.4921259850000001" footer="0.4921259850000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -836,24 +898,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -872,35 +935,59 @@
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
+    <row r="2" spans="1:7" s="2" customFormat="1">
       <c r="A2" s="3">
+        <v>40429</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1">
+      <c r="A3" s="3">
         <v>40443</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="4">
         <v>5</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E3" s="4">
         <v>15</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
+      <c r="G3" s="4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" s="4" customFormat="1">
-      <c r="A3" s="3">
+    <row r="4" spans="1:7">
+      <c r="A4" s="3">
         <v>40457</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
-        <v>40471</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -908,9 +995,9 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="3">
-        <v>40485</v>
+        <v>40471</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -918,9 +1005,9 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="3">
-        <v>40499</v>
+        <v>40485</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -928,9 +1015,9 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="3">
-        <v>40513</v>
+        <v>40499</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -938,8 +1025,10 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>40513</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -947,11 +1036,11 @@
       <c r="F8" s="4"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -961,14 +1050,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
   <headerFooter alignWithMargins="0"/>
@@ -981,14 +1069,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
big chart atualizado com os testes
</commit_message>
<xml_diff>
--- a/documentos/bigChart/BigChartProjeto.xlsx
+++ b/documentos/bigChart/BigChartProjeto.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="11640"/>
   </bookViews>
@@ -122,8 +122,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:lang val="pt-BR"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -165,28 +164,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40429.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40443.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40457.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40471.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40485.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40499.0</c:v>
+                  <c:v>40499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40513.0</c:v>
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -198,13 +197,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -251,28 +250,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40429.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40443.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40457.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40471.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40485.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40499.0</c:v>
+                  <c:v>40499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40513.0</c:v>
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -284,13 +283,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -314,28 +313,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40429.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40443.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40457.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40471.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40485.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40499.0</c:v>
+                  <c:v>40499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40513.0</c:v>
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,13 +346,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -377,28 +376,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40429.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40443.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40457.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40471.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40485.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40499.0</c:v>
+                  <c:v>40499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40513.0</c:v>
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,13 +409,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,28 +439,28 @@
             <c:numRef>
               <c:f>Plan1!$A$2:$A$8</c:f>
               <c:numCache>
-                <c:formatCode>dd.mm.yy</c:formatCode>
+                <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40429.0</c:v>
+                  <c:v>40429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40443.0</c:v>
+                  <c:v>40443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40457.0</c:v>
+                  <c:v>40457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40471.0</c:v>
+                  <c:v>40471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40485.0</c:v>
+                  <c:v>40485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40499.0</c:v>
+                  <c:v>40499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40513.0</c:v>
+                  <c:v>40513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -473,13 +472,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,24 +497,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="506123480"/>
-        <c:axId val="506127080"/>
+        <c:axId val="55511296"/>
+        <c:axId val="55521280"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="506123480"/>
+        <c:axId val="55511296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,21 +529,21 @@
             <a:pPr>
               <a:defRPr lang="pt-BR"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506127080"/>
+        <c:crossAx val="55521280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="14.0"/>
+        <c:majorUnit val="14"/>
         <c:majorTimeUnit val="days"/>
-        <c:minorUnit val="7.0"/>
+        <c:minorUnit val="7"/>
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="506127080"/>
+        <c:axId val="55521280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,10 +559,10 @@
             <a:pPr>
               <a:defRPr lang="pt-BR"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506123480"/>
+        <c:crossAx val="55511296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -579,7 +578,7 @@
             <a:pPr rtl="0">
               <a:defRPr lang="pt-BR"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -589,7 +588,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.984251969" l="0.787401575" r="0.787401575" t="0.984251969" header="0.492125985" footer="0.492125985"/>
+    <c:pageMargins b="0.98425196899999989" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999989" header="0.4921259850000001" footer="0.4921259850000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -916,22 +915,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1">
@@ -1014,7 +1013,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="5">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4">
         <v>27</v>
@@ -1080,12 +1079,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
@@ -1099,12 +1098,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>

</xml_diff>